<commit_message>
subi la nueva estimacion
</commit_message>
<xml_diff>
--- a/Proyecto final/SeguimientoExposiciones.xlsx
+++ b/Proyecto final/SeguimientoExposiciones.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="15255" windowHeight="6150"/>
@@ -11,12 +11,12 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>Nro Exposicion</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>No teniamos definida la tecnica. Inconsistencia en los dichos del equipo</t>
+  </si>
+  <si>
+    <t>Exposicion oral /entrega final De Exposicion</t>
   </si>
 </sst>
 </file>
@@ -402,16 +405,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" customWidth="1"/>
+    <col min="3" max="3" width="50.28515625" customWidth="1"/>
     <col min="6" max="6" width="41.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -507,6 +510,20 @@
       </c>
       <c r="F5" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>41051</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
criticas de la expo expo22052012.txt
</commit_message>
<xml_diff>
--- a/Proyecto final/SeguimientoExposiciones.xlsx
+++ b/Proyecto final/SeguimientoExposiciones.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Nro Exposicion</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>entregamo el informe y expo oral</t>
+  </si>
+  <si>
+    <t>liberal</t>
+  </si>
+  <si>
+    <t>kapica</t>
+  </si>
+  <si>
+    <t>peker</t>
   </si>
 </sst>
 </file>
@@ -411,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -424,7 +433,7 @@
     <col min="6" max="6" width="41.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -443,8 +452,17 @@
       <c r="F1" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
@@ -464,7 +482,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>2</v>
       </c>
@@ -478,7 +496,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>3</v>
       </c>
@@ -498,7 +516,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>4</v>
       </c>
@@ -518,7 +536,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>5</v>
       </c>
@@ -536,6 +554,15 @@
       </c>
       <c r="F6" t="s">
         <v>17</v>
+      </c>
+      <c r="G6">
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <v>9</v>
+      </c>
+      <c r="I6">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>